<commit_message>
completed settings for export
</commit_message>
<xml_diff>
--- a/PEC2mat_settings.xlsx
+++ b/PEC2mat_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dl\Documents\GitHub\MSE_Thesis\battery_testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dl\Documents\GitHub\PEC2mat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0191AB-E738-4FEB-B696-52C4AF7CC235}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40B3277-2776-45B8-B7F0-EB97CC721A91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="1665" windowWidth="11400" windowHeight="16155" xr2:uid="{5B2798EE-F1EB-4EAF-9258-322B38E8B60A}"/>
+    <workbookView xWindow="1294" yWindow="120" windowWidth="19063" windowHeight="7191" xr2:uid="{5B2798EE-F1EB-4EAF-9258-322B38E8B60A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>Cell ID</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Station Temperature (°C)</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Charge Energy Density (Wh/kg)</t>
+  </si>
+  <si>
+    <t>Discharge Energy Density (Wh/kg)</t>
   </si>
 </sst>
 </file>
@@ -177,12 +186,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -197,9 +224,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,19 +544,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926900DB-7D90-4530-B5C1-8A9BA07547EB}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -534,289 +564,313 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{F82823D5-5DDB-4FC9-8A6F-25C3FBC8042E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B36">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B39">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
added first test case for struct with automatic export
</commit_message>
<xml_diff>
--- a/PEC2mat_settings.xlsx
+++ b/PEC2mat_settings.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dl\Documents\GitHub\PEC2mat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40B3277-2776-45B8-B7F0-EB97CC721A91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AD4B93-7602-471C-8EF2-8F44E768B3D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1294" yWindow="120" windowWidth="19063" windowHeight="7191" xr2:uid="{5B2798EE-F1EB-4EAF-9258-322B38E8B60A}"/>
+    <workbookView xWindow="5445" yWindow="6150" windowWidth="20865" windowHeight="12990" xr2:uid="{5B2798EE-F1EB-4EAF-9258-322B38E8B60A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="55">
   <si>
     <t>Cell ID</t>
   </si>
@@ -163,6 +163,42 @@
   </si>
   <si>
     <t>Discharge Energy Density (Wh/kg)</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Default PEC variable</t>
+  </si>
+  <si>
+    <t>User defined variable</t>
+  </si>
+  <si>
+    <t>PT-100_2 (°C)</t>
+  </si>
+  <si>
+    <t>PT-100_3 (°C)</t>
+  </si>
+  <si>
+    <t>PT-100_4 (°C)</t>
+  </si>
+  <si>
+    <t>PT-100_5 (°C)</t>
+  </si>
+  <si>
+    <t>PT-100_6 (°C)</t>
+  </si>
+  <si>
+    <t>PT-100_7 (°C)</t>
+  </si>
+  <si>
+    <t>PT-100_8 (°C)</t>
+  </si>
+  <si>
+    <t>PT-100_9 (°C)</t>
+  </si>
+  <si>
+    <t>PT-100_10 (°C)</t>
   </si>
 </sst>
 </file>
@@ -186,30 +222,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -224,12 +242,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,336 +560,549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926900DB-7D90-4530-B5C1-8A9BA07547EB}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A29" s="4" t="s">
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B39" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A31" s="2" t="s">
+      <c r="C39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B40" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A32" s="2" t="s">
+      <c r="C40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A33" s="2" t="s">
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B42" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A35" s="2" t="s">
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A36" s="2" t="s">
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A37" s="2" t="s">
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A39" s="2" t="s">
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B39" t="s">
-        <v>8</v>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{F82823D5-5DDB-4FC9-8A6F-25C3FBC8042E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B39">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:C1" xr:uid="{6E1E401C-1B1B-4DAF-B038-F4214D7AA558}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
restructured settings.xlsx by introducing variables to remove NaNs
</commit_message>
<xml_diff>
--- a/PEC2mat_settings.xlsx
+++ b/PEC2mat_settings.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dl\Documents\GitHub\PEC2mat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AD4B93-7602-471C-8EF2-8F44E768B3D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9828773F-76D4-4359-97C3-BA88766B2C0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="6150" windowWidth="20865" windowHeight="12990" xr2:uid="{5B2798EE-F1EB-4EAF-9258-322B38E8B60A}"/>
+    <workbookView xWindow="7965" yWindow="9495" windowWidth="22995" windowHeight="6945" activeTab="1" xr2:uid="{5B2798EE-F1EB-4EAF-9258-322B38E8B60A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Variables" sheetId="1" r:id="rId1"/>
+    <sheet name="removeNaNs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">removeNaNs!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="57">
   <si>
     <t>Cell ID</t>
   </si>
@@ -199,6 +201,12 @@
   </si>
   <si>
     <t>PT-100_10 (°C)</t>
+  </si>
+  <si>
+    <t>Ctr</t>
+  </si>
+  <si>
+    <t>PT_100</t>
   </si>
 </sst>
 </file>
@@ -562,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926900DB-7D90-4530-B5C1-8A9BA07547EB}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:C48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,4 +1114,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F129771-BFCD-469A-9868-E696F177908B}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1" xr:uid="{91FCE369-91ED-4995-96FB-0694376FE96F}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>